<commit_message>
93 testcases (icl GUI)
</commit_message>
<xml_diff>
--- a/TCs/Sơn_Testcase.xlsx
+++ b/TCs/Sơn_Testcase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KCPM\Project\Test Document\KCPM-Reports\TCs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1106E45-855A-4777-9217-D808BD392530}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FA1281-FC81-4FC5-B53E-2D1BEE36C79E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="518">
   <si>
     <t>No.</t>
   </si>
@@ -1998,6 +1998,218 @@
 6. Nhập lại mật khẩu: "1234567"
 7. Click Đăng ký</t>
   </si>
+  <si>
+    <t>Nhập email chứa ký tự khoảng trắng ở cuối</t>
+  </si>
+  <si>
+    <t>1. Click vào "Đăng nhập/Đăng ký" trên thanh navbar
+2. Click vào "Tạo tại khoản"
+3. Nhập họ tên, số điện thoại, ngày sinh, giới tính
+4. Nhập email chứa khoảng trắng ở đầu:
+ "ntsonnn10@gmail.com       "
+5. Nhập mật khẩu: "1234567"
+6. Nhập lại mật khẩu: "1234567"
+7. Click Đăng ký</t>
+  </si>
+  <si>
+    <t>1. Đăng ký tài khoản thành công
+2. Hiển thị thông báo "You are now registered and can log in :)"
+3. Có thể đăng nhập vào trang web bằng email đã lược bỏ khoảng trắng ở cuối: "ntsonnn10@gmail.com"</t>
+  </si>
+  <si>
+    <t>F015-T022</t>
+  </si>
+  <si>
+    <t>F015-T023</t>
+  </si>
+  <si>
+    <t>F015-T024</t>
+  </si>
+  <si>
+    <t>F015-T025</t>
+  </si>
+  <si>
+    <t>F015-T026</t>
+  </si>
+  <si>
+    <t>F015-T027</t>
+  </si>
+  <si>
+    <t>F015-T028</t>
+  </si>
+  <si>
+    <t>F015-T029</t>
+  </si>
+  <si>
+    <t>F017-T018</t>
+  </si>
+  <si>
+    <t>F017-T019</t>
+  </si>
+  <si>
+    <t>F017-T020</t>
+  </si>
+  <si>
+    <t>F017-T021</t>
+  </si>
+  <si>
+    <t>F017-T022</t>
+  </si>
+  <si>
+    <t>F018-T001</t>
+  </si>
+  <si>
+    <t>Truy cập vào url trang thông tin cá nhân khi chưa đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Nhập đường dẫn tới trang quản lý thông tin cá nhân vào thanh url của trình duyệt:
+https://e-customer.herokuapp.com/update-account-info.html</t>
+  </si>
+  <si>
+    <t>Truy cập vào url trang thông tin cá nhân khi đã đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Chưa đăng nhập vào trang web.
+2. Trình duyệt không lưu bất kì thông tin cookie hay session nào của trang web</t>
+  </si>
+  <si>
+    <t>1. Truy cập tới trang quản lý thông tin cá nhân của người dùng</t>
+  </si>
+  <si>
+    <t>F018-T002</t>
+  </si>
+  <si>
+    <t>F018-T003</t>
+  </si>
+  <si>
+    <t>F018-T004</t>
+  </si>
+  <si>
+    <t>F018-T005</t>
+  </si>
+  <si>
+    <t>F018-T006</t>
+  </si>
+  <si>
+    <t>F018-T007</t>
+  </si>
+  <si>
+    <t>F018-T008</t>
+  </si>
+  <si>
+    <t>F018-T009</t>
+  </si>
+  <si>
+    <t>F018-T010</t>
+  </si>
+  <si>
+    <t>1. Không thể truy cập trang thông tin cá nhân
+2. Trang web redirect tới trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>Truy cập vào trang Thay đổi mật khẩu khi chưa đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Nhập đường dẫn tới trang quản lý thông tin cá nhân vào thanh url của trình duyệt:
+https://e-customer.herokuapp.com/update-account-password.html</t>
+  </si>
+  <si>
+    <t>1. Không thể truy cập trang Thay đổi mật khẩu
+2. Trang web redirect tới trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>Truy cập vào trang Thay đổi mật khẩu khi đã đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Truy cập tới trang thay đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Truy cập vào trang thanh toán giỏ hàng của người dùng khi chưa đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Không thể truy cập trang Thanh toán giỏ hàng
+2. Trang web redirect tới trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>1. Nhập đường dẫn tới trang Thanh toán giỏ hàng vào thanh url của trình duyệt:
+https://e-customer.herokuapp.com/checkout.html</t>
+  </si>
+  <si>
+    <t>Truy cập vào trang thanh toán giỏ hàng của người dùng khi đã đăng nhập</t>
+  </si>
+  <si>
+    <t>1. Truy cập tới trang thanh toán giỏ hàng</t>
+  </si>
+  <si>
+    <t>Sử dụng nút Back của trình duyệt để quay về trang Quản lý thông tin cá nhân sau khi đăng xuất</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập vào hệ thống với email vào password hợp lệ
+2. Truy cập trang quản lý thông tin cá nhân
+3. Click vào Đăng xuất trên thanh navbar
+4. Click vào nút Back của trình duyệt</t>
+  </si>
+  <si>
+    <t>1. Không thể quay lại trang quản lý thông tin cá nhân
+2. Trang web redirect về trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>1. Vẫn có thể quay lại trang quản lý thông tin cá nhân</t>
+  </si>
+  <si>
+    <t>Sử dụng nút Back của trình duyệt để quay về trang Đổi mật khẩu sau khi đăng xuất</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập vào hệ thống với email vào password hợp lệ
+2. Truy cập trang Thay đổi mật khẩu
+3. Click vào Đăng xuất trên thanh navbar
+4. Click vào nút Back của trình duyệt</t>
+  </si>
+  <si>
+    <t>1. Không thể quay lại trang thay đổi mật khẩu
+2. Trang web redirect về trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>1. Vẫn có thể quay lại trang Thay đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Sử dụng nút Back của trình duyệt để quay về trang Thanh toán giỏ hàng sau khi đăng xuất</t>
+  </si>
+  <si>
+    <t>1. Đăng nhập vào hệ thống với email vào password hợp lệ
+2. Click vào icon Giỏ hàng trên thanh navbar
+3. Click vào nút Thanh Toán
+4. Click vào Đăng xuất trên thanh navbar
+5. Click vào nút Back của trình duyệt</t>
+  </si>
+  <si>
+    <t>1. Không thể quay lại trang Thanh toán giỏ hàng
+2. Trang web redirect về trang đăng nhập
+3. Thông báo "You need log in to view this resource"</t>
+  </si>
+  <si>
+    <t>1. Vẫn có thể quay lại trang Thanh toán giỏ hàng</t>
+  </si>
+  <si>
+    <t>Người dùng đã đăng nhập truy cập vào url dành cho Admin</t>
+  </si>
+  <si>
+    <t>1. Đã đăng nhập tài khoản người dùng</t>
+  </si>
+  <si>
+    <t>1. Nhập đường dẫn tới trang quản lý của Admin vào thanh url của trình duyệt:
+https://e-customer.herokuapp.com/admin-home.html#
+2. Enter</t>
+  </si>
+  <si>
+    <t>1. Không thể truy cập trang quản lý của Admin
+2. Trang web redirect về trang chủ dành cho người dùng</t>
+  </si>
 </sst>
 </file>
 
@@ -3334,7 +3546,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A2:AA111" headerRowCount="0" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table_2" displayName="Table_2" ref="A2:AA112" headerRowCount="0" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27">
   <tableColumns count="27">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="26"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="25"/>
@@ -3632,7 +3844,7 @@
   <dimension ref="A1:E998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7753,10 +7965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AA1007"/>
+  <dimension ref="A1:AA1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B48" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J49" sqref="J49"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7873,7 +8085,7 @@
       <c r="Z2" s="94"/>
       <c r="AA2" s="94"/>
     </row>
-    <row r="3" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <v>1</v>
       </c>
@@ -7924,7 +8136,7 @@
       <c r="Z3" s="14"/>
       <c r="AA3" s="14"/>
     </row>
-    <row r="4" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <v>2</v>
       </c>
@@ -7975,7 +8187,7 @@
       <c r="Z4" s="14"/>
       <c r="AA4" s="14"/>
     </row>
-    <row r="5" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
         <v>3</v>
       </c>
@@ -8026,7 +8238,7 @@
       <c r="Z5" s="14"/>
       <c r="AA5" s="14"/>
     </row>
-    <row r="6" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
         <v>4</v>
       </c>
@@ -8077,7 +8289,7 @@
       <c r="Z6" s="14"/>
       <c r="AA6" s="14"/>
     </row>
-    <row r="7" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70">
         <v>5</v>
       </c>
@@ -8128,7 +8340,7 @@
       <c r="Z7" s="14"/>
       <c r="AA7" s="14"/>
     </row>
-    <row r="8" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
         <v>6</v>
       </c>
@@ -8179,7 +8391,7 @@
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
     </row>
-    <row r="9" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
         <v>7</v>
       </c>
@@ -8230,7 +8442,7 @@
       <c r="Z9" s="14"/>
       <c r="AA9" s="14"/>
     </row>
-    <row r="10" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="70">
         <v>8</v>
       </c>
@@ -8283,7 +8495,7 @@
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
     </row>
-    <row r="11" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="70">
         <v>9</v>
       </c>
@@ -8336,7 +8548,7 @@
       <c r="Z11" s="14"/>
       <c r="AA11" s="14"/>
     </row>
-    <row r="12" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="70">
         <v>10</v>
       </c>
@@ -8389,7 +8601,7 @@
       <c r="Z12" s="14"/>
       <c r="AA12" s="14"/>
     </row>
-    <row r="13" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="70">
         <v>11</v>
       </c>
@@ -8442,7 +8654,7 @@
       <c r="Z13" s="14"/>
       <c r="AA13" s="14"/>
     </row>
-    <row r="14" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="70">
         <v>12</v>
       </c>
@@ -8495,7 +8707,7 @@
       <c r="Z14" s="14"/>
       <c r="AA14" s="14"/>
     </row>
-    <row r="15" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="70">
         <v>13</v>
       </c>
@@ -8548,7 +8760,7 @@
       <c r="Z15" s="15"/>
       <c r="AA15" s="15"/>
     </row>
-    <row r="16" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="70">
         <v>14</v>
       </c>
@@ -8601,7 +8813,7 @@
       <c r="Z16" s="18"/>
       <c r="AA16" s="18"/>
     </row>
-    <row r="17" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="70">
         <v>15</v>
       </c>
@@ -8654,7 +8866,7 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="16"/>
     </row>
-    <row r="18" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="70">
         <v>16</v>
       </c>
@@ -8707,7 +8919,7 @@
       <c r="Z18" s="16"/>
       <c r="AA18" s="16"/>
     </row>
-    <row r="19" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="70">
         <v>17</v>
       </c>
@@ -8760,7 +8972,7 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="16"/>
     </row>
-    <row r="20" spans="1:27" ht="102.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="102.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="70">
         <v>18</v>
       </c>
@@ -8813,7 +9025,7 @@
       <c r="Z20" s="14"/>
       <c r="AA20" s="14"/>
     </row>
-    <row r="21" spans="1:27" ht="102.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="102.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="70">
         <v>19</v>
       </c>
@@ -8866,7 +9078,7 @@
       <c r="Z21" s="14"/>
       <c r="AA21" s="14"/>
     </row>
-    <row r="22" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="70">
         <v>20</v>
       </c>
@@ -8919,7 +9131,7 @@
       <c r="Z22" s="14"/>
       <c r="AA22" s="14"/>
     </row>
-    <row r="23" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="70">
         <v>21</v>
       </c>
@@ -8972,7 +9184,7 @@
       <c r="Z23" s="14"/>
       <c r="AA23" s="14"/>
     </row>
-    <row r="24" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="70">
         <v>22</v>
       </c>
@@ -9025,7 +9237,7 @@
       <c r="Z24" s="14"/>
       <c r="AA24" s="14"/>
     </row>
-    <row r="25" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="70">
         <v>23</v>
       </c>
@@ -9078,7 +9290,7 @@
       <c r="Z25" s="14"/>
       <c r="AA25" s="14"/>
     </row>
-    <row r="26" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="70">
         <v>24</v>
       </c>
@@ -9131,7 +9343,7 @@
       <c r="Z26" s="14"/>
       <c r="AA26" s="14"/>
     </row>
-    <row r="27" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="70">
         <v>25</v>
       </c>
@@ -9184,7 +9396,7 @@
       <c r="Z27" s="14"/>
       <c r="AA27" s="14"/>
     </row>
-    <row r="28" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="70">
         <v>26</v>
       </c>
@@ -9237,7 +9449,7 @@
       <c r="Z28" s="14"/>
       <c r="AA28" s="14"/>
     </row>
-    <row r="29" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="70">
         <v>27</v>
       </c>
@@ -9290,7 +9502,7 @@
       <c r="Z29" s="14"/>
       <c r="AA29" s="14"/>
     </row>
-    <row r="30" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="70">
         <v>28</v>
       </c>
@@ -9343,7 +9555,7 @@
       <c r="Z30" s="14"/>
       <c r="AA30" s="14"/>
     </row>
-    <row r="31" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="70">
         <v>29</v>
       </c>
@@ -9396,7 +9608,7 @@
       <c r="Z31" s="14"/>
       <c r="AA31" s="14"/>
     </row>
-    <row r="32" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="70">
         <v>30</v>
       </c>
@@ -9449,7 +9661,7 @@
       <c r="Z32" s="14"/>
       <c r="AA32" s="14"/>
     </row>
-    <row r="33" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="70">
         <v>30</v>
       </c>
@@ -9502,7 +9714,7 @@
       <c r="Z33" s="14"/>
       <c r="AA33" s="14"/>
     </row>
-    <row r="34" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="70">
         <v>31</v>
       </c>
@@ -9555,7 +9767,7 @@
       <c r="Z34" s="14"/>
       <c r="AA34" s="14"/>
     </row>
-    <row r="35" spans="1:27" s="77" customFormat="1" ht="129" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" s="77" customFormat="1" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="70">
         <v>32</v>
       </c>
@@ -9608,7 +9820,7 @@
       <c r="Z35" s="76"/>
       <c r="AA35" s="76"/>
     </row>
-    <row r="36" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="70">
         <v>33</v>
       </c>
@@ -9659,7 +9871,7 @@
       <c r="Z36" s="14"/>
       <c r="AA36" s="14"/>
     </row>
-    <row r="37" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="70">
         <v>34</v>
       </c>
@@ -9712,7 +9924,7 @@
       <c r="Z37" s="14"/>
       <c r="AA37" s="14"/>
     </row>
-    <row r="38" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="70">
         <v>35</v>
       </c>
@@ -9765,7 +9977,7 @@
       <c r="Z38" s="14"/>
       <c r="AA38" s="14"/>
     </row>
-    <row r="39" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="70">
         <v>36</v>
       </c>
@@ -9816,7 +10028,7 @@
       <c r="Z39" s="14"/>
       <c r="AA39" s="14"/>
     </row>
-    <row r="40" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="70">
         <v>37</v>
       </c>
@@ -9867,7 +10079,7 @@
       <c r="Z40" s="14"/>
       <c r="AA40" s="14"/>
     </row>
-    <row r="41" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="70">
         <v>38</v>
       </c>
@@ -9918,7 +10130,7 @@
       <c r="Z41" s="14"/>
       <c r="AA41" s="14"/>
     </row>
-    <row r="42" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="70">
         <v>39</v>
       </c>
@@ -9969,7 +10181,7 @@
       <c r="Z42" s="14"/>
       <c r="AA42" s="14"/>
     </row>
-    <row r="43" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="70">
         <v>40</v>
       </c>
@@ -10020,10 +10232,12 @@
       <c r="Z43" s="14"/>
       <c r="AA43" s="14"/>
     </row>
-    <row r="44" spans="1:27" s="78" customFormat="1" ht="143.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="70"/>
+    <row r="44" spans="1:27" s="78" customFormat="1" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="70">
+        <v>41</v>
+      </c>
       <c r="B44" s="70" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="C44" s="70" t="s">
         <v>14</v>
@@ -10069,10 +10283,12 @@
       <c r="Z44" s="14"/>
       <c r="AA44" s="14"/>
     </row>
-    <row r="45" spans="1:27" s="78" customFormat="1" ht="143.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="70"/>
+    <row r="45" spans="1:27" s="78" customFormat="1" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="70">
+        <v>42</v>
+      </c>
       <c r="B45" s="70" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="C45" s="70" t="s">
         <v>14</v>
@@ -10118,12 +10334,12 @@
       <c r="Z45" s="14"/>
       <c r="AA45" s="14"/>
     </row>
-    <row r="46" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="70">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B46" s="70" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
       <c r="C46" s="70" t="s">
         <v>14</v>
@@ -10169,12 +10385,12 @@
       <c r="Z46" s="14"/>
       <c r="AA46" s="14"/>
     </row>
-    <row r="47" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="70">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B47" s="70" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="C47" s="70" t="s">
         <v>14</v>
@@ -10220,12 +10436,12 @@
       <c r="Z47" s="14"/>
       <c r="AA47" s="14"/>
     </row>
-    <row r="48" spans="1:27" s="78" customFormat="1" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" s="78" customFormat="1" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="70">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B48" s="70" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="C48" s="70" t="s">
         <v>14</v>
@@ -10234,17 +10450,17 @@
         <v>55</v>
       </c>
       <c r="E48" s="71" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="F48" s="70"/>
       <c r="G48" s="71" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="H48" s="71" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="I48" s="71" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="J48" s="71" t="s">
         <v>52</v>
@@ -10271,12 +10487,12 @@
       <c r="Z48" s="14"/>
       <c r="AA48" s="14"/>
     </row>
-    <row r="49" spans="1:27" s="78" customFormat="1" ht="143.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" s="78" customFormat="1" ht="143.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="70">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B49" s="70" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="C49" s="70" t="s">
         <v>14</v>
@@ -10285,20 +10501,20 @@
         <v>55</v>
       </c>
       <c r="E49" s="71" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="F49" s="70"/>
       <c r="G49" s="71" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="H49" s="71" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I49" s="71" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="J49" s="71" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K49" s="70"/>
       <c r="L49" s="70" t="s">
@@ -10322,12 +10538,12 @@
       <c r="Z49" s="14"/>
       <c r="AA49" s="14"/>
     </row>
-    <row r="50" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" s="78" customFormat="1" ht="157.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="70">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B50" s="70" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="C50" s="70" t="s">
         <v>14</v>
@@ -10335,21 +10551,21 @@
       <c r="D50" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="E50" s="70" t="s">
-        <v>251</v>
+      <c r="E50" s="71" t="s">
+        <v>453</v>
       </c>
       <c r="F50" s="70"/>
-      <c r="G50" s="70" t="s">
-        <v>252</v>
-      </c>
-      <c r="H50" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="I50" s="70" t="s">
-        <v>253</v>
-      </c>
-      <c r="J50" s="70" t="s">
-        <v>52</v>
+      <c r="G50" s="71" t="s">
+        <v>454</v>
+      </c>
+      <c r="H50" s="71" t="s">
+        <v>457</v>
+      </c>
+      <c r="I50" s="71" t="s">
+        <v>455</v>
+      </c>
+      <c r="J50" s="71" t="s">
+        <v>60</v>
       </c>
       <c r="K50" s="70"/>
       <c r="L50" s="70" t="s">
@@ -10373,12 +10589,12 @@
       <c r="Z50" s="14"/>
       <c r="AA50" s="14"/>
     </row>
-    <row r="51" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="70">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B51" s="70" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="C51" s="70" t="s">
         <v>14</v>
@@ -10387,20 +10603,20 @@
         <v>55</v>
       </c>
       <c r="E51" s="70" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="F51" s="70"/>
       <c r="G51" s="70" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H51" s="70" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I51" s="70" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="J51" s="70" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K51" s="70"/>
       <c r="L51" s="70" t="s">
@@ -10424,10 +10640,12 @@
       <c r="Z51" s="14"/>
       <c r="AA51" s="14"/>
     </row>
-    <row r="52" spans="1:27" s="78" customFormat="1" ht="214.5" x14ac:dyDescent="0.25">
-      <c r="A52" s="70"/>
+    <row r="52" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="70">
+        <v>49</v>
+      </c>
       <c r="B52" s="70" t="s">
-        <v>254</v>
+        <v>272</v>
       </c>
       <c r="C52" s="70" t="s">
         <v>14</v>
@@ -10435,20 +10653,20 @@
       <c r="D52" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="E52" s="71" t="s">
-        <v>439</v>
+      <c r="E52" s="70" t="s">
+        <v>255</v>
       </c>
       <c r="F52" s="70"/>
-      <c r="G52" s="71" t="s">
-        <v>442</v>
-      </c>
-      <c r="H52" s="71" t="s">
-        <v>443</v>
-      </c>
-      <c r="I52" s="71" t="s">
-        <v>448</v>
-      </c>
-      <c r="J52" s="71" t="s">
+      <c r="G52" s="70" t="s">
+        <v>256</v>
+      </c>
+      <c r="H52" s="70" t="s">
+        <v>257</v>
+      </c>
+      <c r="I52" s="70" t="s">
+        <v>249</v>
+      </c>
+      <c r="J52" s="70" t="s">
         <v>60</v>
       </c>
       <c r="K52" s="70"/>
@@ -10473,10 +10691,12 @@
       <c r="Z52" s="14"/>
       <c r="AA52" s="14"/>
     </row>
-    <row r="53" spans="1:27" s="78" customFormat="1" ht="214.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="70"/>
+    <row r="53" spans="1:27" s="78" customFormat="1" ht="214.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="70">
+        <v>50</v>
+      </c>
       <c r="B53" s="70" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="C53" s="70" t="s">
         <v>14</v>
@@ -10485,17 +10705,17 @@
         <v>55</v>
       </c>
       <c r="E53" s="71" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F53" s="70"/>
       <c r="G53" s="71" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H53" s="71" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="I53" s="71" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="J53" s="71" t="s">
         <v>60</v>
@@ -10522,12 +10742,12 @@
       <c r="Z53" s="14"/>
       <c r="AA53" s="14"/>
     </row>
-    <row r="54" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" s="78" customFormat="1" ht="214.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="70">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B54" s="70" t="s">
-        <v>258</v>
+        <v>347</v>
       </c>
       <c r="C54" s="70" t="s">
         <v>14</v>
@@ -10535,20 +10755,20 @@
       <c r="D54" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="E54" s="70" t="s">
-        <v>259</v>
+      <c r="E54" s="71" t="s">
+        <v>444</v>
       </c>
       <c r="F54" s="70"/>
-      <c r="G54" s="70" t="s">
-        <v>260</v>
-      </c>
-      <c r="H54" s="70" t="s">
-        <v>257</v>
-      </c>
-      <c r="I54" s="70" t="s">
-        <v>249</v>
-      </c>
-      <c r="J54" s="70" t="s">
+      <c r="G54" s="71" t="s">
+        <v>445</v>
+      </c>
+      <c r="H54" s="71" t="s">
+        <v>446</v>
+      </c>
+      <c r="I54" s="71" t="s">
+        <v>447</v>
+      </c>
+      <c r="J54" s="71" t="s">
         <v>60</v>
       </c>
       <c r="K54" s="70"/>
@@ -10573,28 +10793,28 @@
       <c r="Z54" s="14"/>
       <c r="AA54" s="14"/>
     </row>
-    <row r="55" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="70">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B55" s="70" t="s">
-        <v>261</v>
+        <v>348</v>
       </c>
       <c r="C55" s="70" t="s">
         <v>14</v>
       </c>
       <c r="D55" s="70" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="E55" s="70" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="F55" s="70"/>
-      <c r="G55" s="71" t="s">
-        <v>263</v>
+      <c r="G55" s="70" t="s">
+        <v>260</v>
       </c>
       <c r="H55" s="70" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="I55" s="70" t="s">
         <v>249</v>
@@ -10624,12 +10844,12 @@
       <c r="Z55" s="14"/>
       <c r="AA55" s="14"/>
     </row>
-    <row r="56" spans="1:27" s="78" customFormat="1" ht="129" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="70">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B56" s="70" t="s">
-        <v>261</v>
+        <v>356</v>
       </c>
       <c r="C56" s="70" t="s">
         <v>14</v>
@@ -10637,12 +10857,12 @@
       <c r="D56" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="71" t="s">
-        <v>440</v>
+      <c r="E56" s="70" t="s">
+        <v>262</v>
       </c>
       <c r="F56" s="70"/>
       <c r="G56" s="71" t="s">
-        <v>441</v>
+        <v>263</v>
       </c>
       <c r="H56" s="70" t="s">
         <v>264</v>
@@ -10675,34 +10895,34 @@
       <c r="Z56" s="14"/>
       <c r="AA56" s="14"/>
     </row>
-    <row r="57" spans="1:27" ht="129" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" s="78" customFormat="1" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="70">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B57" s="70" t="s">
-        <v>265</v>
+        <v>463</v>
       </c>
       <c r="C57" s="70" t="s">
         <v>14</v>
       </c>
       <c r="D57" s="70" t="s">
-        <v>55</v>
-      </c>
-      <c r="E57" s="70" t="s">
-        <v>266</v>
+        <v>118</v>
+      </c>
+      <c r="E57" s="71" t="s">
+        <v>440</v>
       </c>
       <c r="F57" s="70"/>
-      <c r="G57" s="70" t="s">
-        <v>267</v>
+      <c r="G57" s="71" t="s">
+        <v>441</v>
       </c>
       <c r="H57" s="70" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="I57" s="70" t="s">
-        <v>268</v>
+        <v>249</v>
       </c>
       <c r="J57" s="70" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K57" s="70"/>
       <c r="L57" s="70" t="s">
@@ -10726,31 +10946,31 @@
       <c r="Z57" s="14"/>
       <c r="AA57" s="14"/>
     </row>
-    <row r="58" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="129" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="70">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B58" s="70" t="s">
-        <v>269</v>
+        <v>464</v>
       </c>
       <c r="C58" s="70" t="s">
         <v>14</v>
       </c>
       <c r="D58" s="70" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="E58" s="70" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F58" s="70"/>
       <c r="G58" s="70" t="s">
-        <v>271</v>
-      </c>
-      <c r="H58" s="71" t="s">
-        <v>379</v>
-      </c>
-      <c r="I58" s="71" t="s">
-        <v>379</v>
+        <v>267</v>
+      </c>
+      <c r="H58" s="70" t="s">
+        <v>268</v>
+      </c>
+      <c r="I58" s="70" t="s">
+        <v>268</v>
       </c>
       <c r="J58" s="70" t="s">
         <v>52</v>
@@ -10760,7 +10980,7 @@
         <v>53</v>
       </c>
       <c r="M58" s="72">
-        <v>44203</v>
+        <v>44202</v>
       </c>
       <c r="N58" s="70"/>
       <c r="O58" s="70"/>
@@ -10777,12 +10997,12 @@
       <c r="Z58" s="14"/>
       <c r="AA58" s="14"/>
     </row>
-    <row r="59" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="70">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B59" s="70" t="s">
-        <v>272</v>
+        <v>465</v>
       </c>
       <c r="C59" s="70" t="s">
         <v>14</v>
@@ -10791,20 +11011,20 @@
         <v>167</v>
       </c>
       <c r="E59" s="70" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="F59" s="70"/>
       <c r="G59" s="70" t="s">
-        <v>274</v>
-      </c>
-      <c r="H59" s="70" t="s">
-        <v>275</v>
-      </c>
-      <c r="I59" s="70" t="s">
-        <v>276</v>
+        <v>271</v>
+      </c>
+      <c r="H59" s="71" t="s">
+        <v>379</v>
+      </c>
+      <c r="I59" s="71" t="s">
+        <v>379</v>
       </c>
       <c r="J59" s="70" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="K59" s="70"/>
       <c r="L59" s="70" t="s">
@@ -10828,12 +11048,12 @@
       <c r="Z59" s="14"/>
       <c r="AA59" s="14"/>
     </row>
-    <row r="60" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="70">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B60" s="70" t="s">
-        <v>277</v>
+        <v>466</v>
       </c>
       <c r="C60" s="70" t="s">
         <v>14</v>
@@ -10842,20 +11062,20 @@
         <v>167</v>
       </c>
       <c r="E60" s="70" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="F60" s="70"/>
       <c r="G60" s="70" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="H60" s="70" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="I60" s="70" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="J60" s="70" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="K60" s="70"/>
       <c r="L60" s="70" t="s">
@@ -10879,12 +11099,12 @@
       <c r="Z60" s="14"/>
       <c r="AA60" s="14"/>
     </row>
-    <row r="61" spans="1:27" ht="72" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="70">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B61" s="70" t="s">
-        <v>347</v>
+        <v>467</v>
       </c>
       <c r="C61" s="70" t="s">
         <v>14</v>
@@ -10892,20 +11112,20 @@
       <c r="D61" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="E61" s="71" t="s">
-        <v>342</v>
+      <c r="E61" s="70" t="s">
+        <v>278</v>
       </c>
       <c r="F61" s="70"/>
-      <c r="G61" s="71" t="s">
-        <v>343</v>
-      </c>
-      <c r="H61" s="71" t="s">
-        <v>344</v>
-      </c>
-      <c r="I61" s="71" t="s">
-        <v>344</v>
-      </c>
-      <c r="J61" s="71" t="s">
+      <c r="G61" s="70" t="s">
+        <v>279</v>
+      </c>
+      <c r="H61" s="70" t="s">
+        <v>280</v>
+      </c>
+      <c r="I61" s="70" t="s">
+        <v>280</v>
+      </c>
+      <c r="J61" s="70" t="s">
         <v>52</v>
       </c>
       <c r="K61" s="70"/>
@@ -10930,12 +11150,12 @@
       <c r="Z61" s="14"/>
       <c r="AA61" s="14"/>
     </row>
-    <row r="62" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="72" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="70">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B62" s="70" t="s">
-        <v>348</v>
+        <v>468</v>
       </c>
       <c r="C62" s="70" t="s">
         <v>14</v>
@@ -10944,19 +11164,19 @@
         <v>167</v>
       </c>
       <c r="E62" s="71" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="F62" s="70"/>
       <c r="G62" s="71" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="H62" s="71" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I62" s="71" t="s">
-        <v>346</v>
-      </c>
-      <c r="J62" s="70" t="s">
+        <v>344</v>
+      </c>
+      <c r="J62" s="71" t="s">
         <v>52</v>
       </c>
       <c r="K62" s="70"/>
@@ -10981,125 +11201,123 @@
       <c r="Z62" s="14"/>
       <c r="AA62" s="14"/>
     </row>
-    <row r="63" spans="1:27" s="77" customFormat="1" ht="86.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="73">
-        <v>53</v>
-      </c>
-      <c r="B63" s="73" t="s">
-        <v>356</v>
-      </c>
-      <c r="C63" s="73" t="s">
+    <row r="63" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="70">
+        <v>60</v>
+      </c>
+      <c r="B63" s="70" t="s">
+        <v>469</v>
+      </c>
+      <c r="C63" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D63" s="74" t="s">
-        <v>200</v>
-      </c>
-      <c r="E63" s="70" t="s">
-        <v>357</v>
+      <c r="D63" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="E63" s="71" t="s">
+        <v>349</v>
       </c>
       <c r="F63" s="70"/>
       <c r="G63" s="71" t="s">
         <v>345</v>
       </c>
-      <c r="H63" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="I63" s="70" t="s">
-        <v>203</v>
+      <c r="H63" s="71" t="s">
+        <v>346</v>
+      </c>
+      <c r="I63" s="71" t="s">
+        <v>346</v>
       </c>
       <c r="J63" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="K63" s="73"/>
+      <c r="K63" s="70"/>
       <c r="L63" s="70" t="s">
         <v>53</v>
       </c>
       <c r="M63" s="72">
         <v>44203</v>
       </c>
-      <c r="N63" s="73"/>
-      <c r="O63" s="73"/>
-      <c r="P63" s="73"/>
-      <c r="Q63" s="73"/>
-      <c r="R63" s="73"/>
-      <c r="S63" s="73"/>
-      <c r="T63" s="73"/>
-      <c r="U63" s="76"/>
-      <c r="V63" s="76"/>
-      <c r="W63" s="76"/>
-      <c r="X63" s="76"/>
-      <c r="Y63" s="76"/>
-      <c r="Z63" s="76"/>
-      <c r="AA63" s="76"/>
-    </row>
-    <row r="64" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="N63" s="70"/>
+      <c r="O63" s="70"/>
+      <c r="P63" s="70"/>
+      <c r="Q63" s="70"/>
+      <c r="R63" s="70"/>
+      <c r="S63" s="70"/>
+      <c r="T63" s="70"/>
+      <c r="U63" s="14"/>
+      <c r="V63" s="14"/>
+      <c r="W63" s="14"/>
+      <c r="X63" s="14"/>
+      <c r="Y63" s="14"/>
+      <c r="Z63" s="14"/>
+      <c r="AA63" s="14"/>
+    </row>
+    <row r="64" spans="1:27" s="77" customFormat="1" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="70">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B64" s="70" t="s">
-        <v>358</v>
-      </c>
-      <c r="C64" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="D64" s="70" t="s">
-        <v>55</v>
+        <v>470</v>
+      </c>
+      <c r="C64" s="73" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="74" t="s">
+        <v>200</v>
       </c>
       <c r="E64" s="70" t="s">
-        <v>360</v>
-      </c>
-      <c r="F64" s="70" t="s">
-        <v>359</v>
-      </c>
+        <v>357</v>
+      </c>
+      <c r="F64" s="70"/>
       <c r="G64" s="71" t="s">
-        <v>436</v>
+        <v>345</v>
       </c>
       <c r="H64" s="70" t="s">
-        <v>361</v>
+        <v>203</v>
       </c>
       <c r="I64" s="70" t="s">
-        <v>361</v>
+        <v>203</v>
       </c>
       <c r="J64" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="K64" s="70"/>
+      <c r="K64" s="73"/>
       <c r="L64" s="70" t="s">
         <v>53</v>
       </c>
       <c r="M64" s="72">
         <v>44203</v>
       </c>
-      <c r="N64" s="70"/>
-      <c r="O64" s="70"/>
-      <c r="P64" s="70"/>
-      <c r="Q64" s="70"/>
-      <c r="R64" s="70"/>
-      <c r="S64" s="70"/>
-      <c r="T64" s="70"/>
-      <c r="U64" s="14"/>
-      <c r="V64" s="14"/>
-      <c r="W64" s="14"/>
-      <c r="X64" s="14"/>
-      <c r="Y64" s="14"/>
-      <c r="Z64" s="14"/>
-      <c r="AA64" s="14"/>
-    </row>
-    <row r="65" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+      <c r="N64" s="73"/>
+      <c r="O64" s="73"/>
+      <c r="P64" s="73"/>
+      <c r="Q64" s="73"/>
+      <c r="R64" s="73"/>
+      <c r="S64" s="73"/>
+      <c r="T64" s="73"/>
+      <c r="U64" s="76"/>
+      <c r="V64" s="76"/>
+      <c r="W64" s="76"/>
+      <c r="X64" s="76"/>
+      <c r="Y64" s="76"/>
+      <c r="Z64" s="76"/>
+      <c r="AA64" s="76"/>
+    </row>
+    <row r="65" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="70">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B65" s="70" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="C65" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D65" s="70" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="E65" s="70" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F65" s="70" t="s">
         <v>359</v>
@@ -11108,12 +11326,12 @@
         <v>436</v>
       </c>
       <c r="H65" s="70" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="I65" s="70" t="s">
-        <v>363</v>
-      </c>
-      <c r="J65" s="71" t="s">
+        <v>361</v>
+      </c>
+      <c r="J65" s="70" t="s">
         <v>52</v>
       </c>
       <c r="K65" s="70"/>
@@ -11138,12 +11356,12 @@
       <c r="Z65" s="14"/>
       <c r="AA65" s="14"/>
     </row>
-    <row r="66" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="70">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B66" s="70" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C66" s="70" t="s">
         <v>18</v>
@@ -11151,21 +11369,23 @@
       <c r="D66" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="E66" s="79" t="s">
-        <v>364</v>
-      </c>
-      <c r="F66" s="70"/>
+      <c r="E66" s="70" t="s">
+        <v>362</v>
+      </c>
+      <c r="F66" s="70" t="s">
+        <v>359</v>
+      </c>
       <c r="G66" s="71" t="s">
-        <v>365</v>
-      </c>
-      <c r="H66" s="71" t="s">
-        <v>366</v>
-      </c>
-      <c r="I66" s="71" t="s">
-        <v>367</v>
-      </c>
-      <c r="J66" s="70" t="s">
-        <v>60</v>
+        <v>436</v>
+      </c>
+      <c r="H66" s="70" t="s">
+        <v>363</v>
+      </c>
+      <c r="I66" s="70" t="s">
+        <v>363</v>
+      </c>
+      <c r="J66" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K66" s="70"/>
       <c r="L66" s="70" t="s">
@@ -11189,12 +11409,12 @@
       <c r="Z66" s="14"/>
       <c r="AA66" s="14"/>
     </row>
-    <row r="67" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="70">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B67" s="70" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C67" s="70" t="s">
         <v>18</v>
@@ -11202,21 +11422,21 @@
       <c r="D67" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="71" t="s">
-        <v>377</v>
+      <c r="E67" s="79" t="s">
+        <v>364</v>
       </c>
       <c r="F67" s="70"/>
       <c r="G67" s="71" t="s">
-        <v>436</v>
+        <v>365</v>
       </c>
       <c r="H67" s="71" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="I67" s="71" t="s">
-        <v>378</v>
-      </c>
-      <c r="J67" s="71" t="s">
-        <v>52</v>
+        <v>367</v>
+      </c>
+      <c r="J67" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="K67" s="70"/>
       <c r="L67" s="70" t="s">
@@ -11240,33 +11460,31 @@
       <c r="Z67" s="14"/>
       <c r="AA67" s="14"/>
     </row>
-    <row r="68" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="70">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B68" s="70" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C68" s="70" t="s">
         <v>18</v>
       </c>
-      <c r="D68" s="71" t="s">
-        <v>55</v>
+      <c r="D68" s="70" t="s">
+        <v>167</v>
       </c>
       <c r="E68" s="71" t="s">
-        <v>380</v>
-      </c>
-      <c r="F68" s="71" t="s">
-        <v>381</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="F68" s="70"/>
       <c r="G68" s="71" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="H68" s="71" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="I68" s="71" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="J68" s="71" t="s">
         <v>52</v>
@@ -11293,12 +11511,12 @@
       <c r="Z68" s="14"/>
       <c r="AA68" s="14"/>
     </row>
-    <row r="69" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="70">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="B69" s="70" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C69" s="70" t="s">
         <v>18</v>
@@ -11307,17 +11525,19 @@
         <v>55</v>
       </c>
       <c r="E69" s="71" t="s">
-        <v>383</v>
-      </c>
-      <c r="F69" s="70"/>
+        <v>380</v>
+      </c>
+      <c r="F69" s="71" t="s">
+        <v>381</v>
+      </c>
       <c r="G69" s="71" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H69" s="71" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I69" s="71" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="J69" s="71" t="s">
         <v>52</v>
@@ -11344,12 +11564,12 @@
       <c r="Z69" s="14"/>
       <c r="AA69" s="14"/>
     </row>
-    <row r="70" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="70">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B70" s="70" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C70" s="70" t="s">
         <v>18</v>
@@ -11358,17 +11578,17 @@
         <v>55</v>
       </c>
       <c r="E70" s="71" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F70" s="70"/>
       <c r="G70" s="71" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H70" s="71" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I70" s="71" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="J70" s="71" t="s">
         <v>52</v>
@@ -11395,12 +11615,12 @@
       <c r="Z70" s="14"/>
       <c r="AA70" s="14"/>
     </row>
-    <row r="71" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="70">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B71" s="70" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C71" s="70" t="s">
         <v>18</v>
@@ -11409,20 +11629,20 @@
         <v>55</v>
       </c>
       <c r="E71" s="71" t="s">
-        <v>402</v>
+        <v>385</v>
       </c>
       <c r="F71" s="70"/>
       <c r="G71" s="71" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H71" s="71" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I71" s="71" t="s">
         <v>386</v>
       </c>
-      <c r="J71" s="70" t="s">
-        <v>60</v>
+      <c r="J71" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K71" s="70"/>
       <c r="L71" s="70" t="s">
@@ -11446,31 +11666,31 @@
       <c r="Z71" s="14"/>
       <c r="AA71" s="14"/>
     </row>
-    <row r="72" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="70">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B72" s="70" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C72" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D72" s="71" t="s">
-        <v>167</v>
+        <v>55</v>
       </c>
       <c r="E72" s="71" t="s">
-        <v>388</v>
+        <v>402</v>
       </c>
       <c r="F72" s="70"/>
       <c r="G72" s="71" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H72" s="71" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I72" s="71" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="J72" s="70" t="s">
         <v>60</v>
@@ -11497,34 +11717,34 @@
       <c r="Z72" s="14"/>
       <c r="AA72" s="14"/>
     </row>
-    <row r="73" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="70">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B73" s="70" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C73" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D73" s="71" t="s">
-        <v>391</v>
+        <v>167</v>
       </c>
       <c r="E73" s="71" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="F73" s="70"/>
       <c r="G73" s="71" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H73" s="71" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="I73" s="71" t="s">
-        <v>393</v>
-      </c>
-      <c r="J73" s="71" t="s">
-        <v>52</v>
+        <v>390</v>
+      </c>
+      <c r="J73" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="K73" s="70"/>
       <c r="L73" s="70" t="s">
@@ -11548,25 +11768,25 @@
       <c r="Z73" s="14"/>
       <c r="AA73" s="14"/>
     </row>
-    <row r="74" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="70">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B74" s="70" t="s">
-        <v>409</v>
+        <v>376</v>
       </c>
       <c r="C74" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D74" s="71" t="s">
-        <v>55</v>
+        <v>391</v>
       </c>
       <c r="E74" s="71" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F74" s="70"/>
       <c r="G74" s="71" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H74" s="71" t="s">
         <v>393</v>
@@ -11599,12 +11819,12 @@
       <c r="Z74" s="14"/>
       <c r="AA74" s="14"/>
     </row>
-    <row r="75" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="70">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B75" s="70" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C75" s="70" t="s">
         <v>18</v>
@@ -11613,17 +11833,17 @@
         <v>55</v>
       </c>
       <c r="E75" s="71" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F75" s="70"/>
       <c r="G75" s="71" t="s">
-        <v>396</v>
+        <v>429</v>
       </c>
       <c r="H75" s="71" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="I75" s="71" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J75" s="71" t="s">
         <v>52</v>
@@ -11650,12 +11870,12 @@
       <c r="Z75" s="14"/>
       <c r="AA75" s="14"/>
     </row>
-    <row r="76" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" ht="57.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="70">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B76" s="70" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C76" s="70" t="s">
         <v>18</v>
@@ -11664,17 +11884,17 @@
         <v>55</v>
       </c>
       <c r="E76" s="71" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F76" s="70"/>
       <c r="G76" s="71" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="H76" s="71" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I76" s="71" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="J76" s="71" t="s">
         <v>52</v>
@@ -11701,12 +11921,12 @@
       <c r="Z76" s="14"/>
       <c r="AA76" s="14"/>
     </row>
-    <row r="77" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="70">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B77" s="70" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C77" s="70" t="s">
         <v>18</v>
@@ -11715,17 +11935,17 @@
         <v>55</v>
       </c>
       <c r="E77" s="71" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="F77" s="70"/>
       <c r="G77" s="71" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H77" s="71" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="I77" s="71" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J77" s="71" t="s">
         <v>52</v>
@@ -11752,12 +11972,12 @@
       <c r="Z77" s="14"/>
       <c r="AA77" s="14"/>
     </row>
-    <row r="78" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="70">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="B78" s="70" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C78" s="70" t="s">
         <v>18</v>
@@ -11766,17 +11986,17 @@
         <v>55</v>
       </c>
       <c r="E78" s="71" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="F78" s="70"/>
       <c r="G78" s="71" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H78" s="71" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I78" s="71" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="J78" s="71" t="s">
         <v>52</v>
@@ -11803,34 +12023,34 @@
       <c r="Z78" s="14"/>
       <c r="AA78" s="14"/>
     </row>
-    <row r="79" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="70">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B79" s="70" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C79" s="70" t="s">
         <v>18</v>
       </c>
       <c r="D79" s="71" t="s">
-        <v>167</v>
-      </c>
-      <c r="E79" s="79" t="s">
-        <v>406</v>
+        <v>55</v>
+      </c>
+      <c r="E79" s="71" t="s">
+        <v>403</v>
       </c>
       <c r="F79" s="70"/>
       <c r="G79" s="71" t="s">
-        <v>407</v>
+        <v>426</v>
       </c>
       <c r="H79" s="71" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="I79" s="71" t="s">
-        <v>367</v>
-      </c>
-      <c r="J79" s="70" t="s">
-        <v>60</v>
+        <v>405</v>
+      </c>
+      <c r="J79" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K79" s="70"/>
       <c r="L79" s="70" t="s">
@@ -11854,12 +12074,12 @@
       <c r="Z79" s="14"/>
       <c r="AA79" s="14"/>
     </row>
-    <row r="80" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="70">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="B80" s="70" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C80" s="70" t="s">
         <v>18</v>
@@ -11867,18 +12087,18 @@
       <c r="D80" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="E80" s="71" t="s">
-        <v>408</v>
+      <c r="E80" s="79" t="s">
+        <v>406</v>
       </c>
       <c r="F80" s="70"/>
       <c r="G80" s="71" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
       <c r="H80" s="71" t="s">
-        <v>389</v>
+        <v>366</v>
       </c>
       <c r="I80" s="71" t="s">
-        <v>390</v>
+        <v>367</v>
       </c>
       <c r="J80" s="70" t="s">
         <v>60</v>
@@ -11905,40 +12125,42 @@
       <c r="Z80" s="14"/>
       <c r="AA80" s="14"/>
     </row>
-    <row r="81" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="70">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B81" s="70" t="s">
-        <v>287</v>
+        <v>415</v>
       </c>
       <c r="C81" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D81" s="71" t="s">
-        <v>55</v>
+        <v>167</v>
       </c>
       <c r="E81" s="71" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F81" s="70"/>
       <c r="G81" s="71" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H81" s="71" t="s">
-        <v>417</v>
+        <v>389</v>
       </c>
       <c r="I81" s="71" t="s">
-        <v>417</v>
-      </c>
-      <c r="J81" s="71" t="s">
-        <v>52</v>
+        <v>390</v>
+      </c>
+      <c r="J81" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="K81" s="70"/>
       <c r="L81" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="M81" s="72"/>
+      <c r="M81" s="72">
+        <v>44203</v>
+      </c>
       <c r="N81" s="70"/>
       <c r="O81" s="70"/>
       <c r="P81" s="70"/>
@@ -11954,31 +12176,31 @@
       <c r="Z81" s="14"/>
       <c r="AA81" s="14"/>
     </row>
-    <row r="82" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" ht="86.25" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="70">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B82" s="70" t="s">
-        <v>287</v>
+        <v>471</v>
       </c>
       <c r="C82" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D82" s="71" t="s">
         <v>55</v>
       </c>
       <c r="E82" s="71" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F82" s="70"/>
       <c r="G82" s="71" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H82" s="71" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I82" s="71" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="J82" s="71" t="s">
         <v>52</v>
@@ -12003,34 +12225,34 @@
       <c r="Z82" s="14"/>
       <c r="AA82" s="14"/>
     </row>
-    <row r="83" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" ht="114.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="70">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="B83" s="70" t="s">
-        <v>287</v>
+        <v>472</v>
       </c>
       <c r="C83" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D83" s="71" t="s">
         <v>55</v>
       </c>
       <c r="E83" s="71" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F83" s="70"/>
       <c r="G83" s="71" t="s">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="H83" s="71" t="s">
-        <v>387</v>
+        <v>419</v>
       </c>
       <c r="I83" s="71" t="s">
         <v>419</v>
       </c>
-      <c r="J83" s="70" t="s">
-        <v>60</v>
+      <c r="J83" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K83" s="70"/>
       <c r="L83" s="70" t="s">
@@ -12052,34 +12274,34 @@
       <c r="Z83" s="14"/>
       <c r="AA83" s="14"/>
     </row>
-    <row r="84" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" ht="100.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="70">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B84" s="70" t="s">
-        <v>287</v>
+        <v>473</v>
       </c>
       <c r="C84" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D84" s="71" t="s">
         <v>55</v>
       </c>
       <c r="E84" s="71" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F84" s="70"/>
       <c r="G84" s="71" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="H84" s="71" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="I84" s="71" t="s">
-        <v>393</v>
-      </c>
-      <c r="J84" s="71" t="s">
-        <v>52</v>
+        <v>419</v>
+      </c>
+      <c r="J84" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="K84" s="70"/>
       <c r="L84" s="70" t="s">
@@ -12101,25 +12323,25 @@
       <c r="Z84" s="14"/>
       <c r="AA84" s="14"/>
     </row>
-    <row r="85" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="70">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B85" s="70" t="s">
-        <v>287</v>
+        <v>474</v>
       </c>
       <c r="C85" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D85" s="71" t="s">
         <v>55</v>
       </c>
       <c r="E85" s="71" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
       <c r="F85" s="70"/>
       <c r="G85" s="71" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="H85" s="71" t="s">
         <v>393</v>
@@ -12150,26 +12372,34 @@
       <c r="Z85" s="14"/>
       <c r="AA85" s="14"/>
     </row>
-    <row r="86" spans="1:27" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A86" s="70">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B86" s="70" t="s">
-        <v>287</v>
+        <v>475</v>
       </c>
       <c r="C86" s="70" t="s">
-        <v>281</v>
+        <v>18</v>
       </c>
       <c r="D86" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="E86" s="71"/>
+      <c r="E86" s="71" t="s">
+        <v>437</v>
+      </c>
       <c r="F86" s="70"/>
-      <c r="G86" s="71"/>
-      <c r="H86" s="70"/>
-      <c r="I86" s="70"/>
-      <c r="J86" s="70" t="s">
-        <v>60</v>
+      <c r="G86" s="71" t="s">
+        <v>438</v>
+      </c>
+      <c r="H86" s="71" t="s">
+        <v>393</v>
+      </c>
+      <c r="I86" s="71" t="s">
+        <v>393</v>
+      </c>
+      <c r="J86" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K86" s="70"/>
       <c r="L86" s="70" t="s">
@@ -12191,32 +12421,36 @@
       <c r="Z86" s="14"/>
       <c r="AA86" s="14"/>
     </row>
-    <row r="87" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A87" s="70">
-        <v>77</v>
-      </c>
-      <c r="B87" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C87" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D87" s="70"/>
-      <c r="E87" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F87" s="70"/>
-      <c r="G87" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H87" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I87" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J87" s="70" t="s">
-        <v>60</v>
+        <v>84</v>
+      </c>
+      <c r="B87" s="71" t="s">
+        <v>476</v>
+      </c>
+      <c r="C87" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E87" s="71" t="s">
+        <v>477</v>
+      </c>
+      <c r="F87" s="71" t="s">
+        <v>480</v>
+      </c>
+      <c r="G87" s="71" t="s">
+        <v>478</v>
+      </c>
+      <c r="H87" s="71" t="s">
+        <v>491</v>
+      </c>
+      <c r="I87" s="71" t="s">
+        <v>491</v>
+      </c>
+      <c r="J87" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K87" s="70"/>
       <c r="L87" s="70" t="s">
@@ -12238,32 +12472,36 @@
       <c r="Z87" s="14"/>
       <c r="AA87" s="14"/>
     </row>
-    <row r="88" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A88" s="70">
-        <v>78</v>
-      </c>
-      <c r="B88" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C88" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D88" s="70"/>
-      <c r="E88" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F88" s="70"/>
-      <c r="G88" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H88" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I88" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J88" s="70" t="s">
-        <v>60</v>
+        <v>85</v>
+      </c>
+      <c r="B88" s="71" t="s">
+        <v>482</v>
+      </c>
+      <c r="C88" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E88" s="71" t="s">
+        <v>479</v>
+      </c>
+      <c r="F88" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="G88" s="71" t="s">
+        <v>478</v>
+      </c>
+      <c r="H88" s="71" t="s">
+        <v>481</v>
+      </c>
+      <c r="I88" s="71" t="s">
+        <v>481</v>
+      </c>
+      <c r="J88" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K88" s="70"/>
       <c r="L88" s="70" t="s">
@@ -12285,32 +12523,36 @@
       <c r="Z88" s="14"/>
       <c r="AA88" s="14"/>
     </row>
-    <row r="89" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A89" s="70">
-        <v>79</v>
-      </c>
-      <c r="B89" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C89" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D89" s="70"/>
-      <c r="E89" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F89" s="70"/>
-      <c r="G89" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H89" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I89" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J89" s="70" t="s">
-        <v>60</v>
+        <v>86</v>
+      </c>
+      <c r="B89" s="71" t="s">
+        <v>483</v>
+      </c>
+      <c r="C89" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D89" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E89" s="71" t="s">
+        <v>492</v>
+      </c>
+      <c r="F89" s="71" t="s">
+        <v>480</v>
+      </c>
+      <c r="G89" s="71" t="s">
+        <v>493</v>
+      </c>
+      <c r="H89" s="71" t="s">
+        <v>494</v>
+      </c>
+      <c r="I89" s="71" t="s">
+        <v>494</v>
+      </c>
+      <c r="J89" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K89" s="70"/>
       <c r="L89" s="70" t="s">
@@ -12332,32 +12574,36 @@
       <c r="Z89" s="14"/>
       <c r="AA89" s="14"/>
     </row>
-    <row r="90" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A90" s="70">
-        <v>80</v>
-      </c>
-      <c r="B90" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C90" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D90" s="70"/>
-      <c r="E90" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F90" s="70"/>
-      <c r="G90" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H90" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I90" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J90" s="70" t="s">
-        <v>60</v>
+        <v>87</v>
+      </c>
+      <c r="B90" s="71" t="s">
+        <v>484</v>
+      </c>
+      <c r="C90" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D90" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E90" s="71" t="s">
+        <v>495</v>
+      </c>
+      <c r="F90" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="G90" s="71" t="s">
+        <v>493</v>
+      </c>
+      <c r="H90" s="71" t="s">
+        <v>496</v>
+      </c>
+      <c r="I90" s="71" t="s">
+        <v>496</v>
+      </c>
+      <c r="J90" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K90" s="70"/>
       <c r="L90" s="70" t="s">
@@ -12379,32 +12625,36 @@
       <c r="Z90" s="14"/>
       <c r="AA90" s="14"/>
     </row>
-    <row r="91" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:27" ht="171.75" x14ac:dyDescent="0.25">
       <c r="A91" s="70">
-        <v>81</v>
-      </c>
-      <c r="B91" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C91" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D91" s="70"/>
-      <c r="E91" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F91" s="70"/>
-      <c r="G91" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H91" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I91" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J91" s="70" t="s">
-        <v>60</v>
+        <v>88</v>
+      </c>
+      <c r="B91" s="71" t="s">
+        <v>485</v>
+      </c>
+      <c r="C91" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D91" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E91" s="71" t="s">
+        <v>497</v>
+      </c>
+      <c r="F91" s="71" t="s">
+        <v>480</v>
+      </c>
+      <c r="G91" s="71" t="s">
+        <v>499</v>
+      </c>
+      <c r="H91" s="71" t="s">
+        <v>498</v>
+      </c>
+      <c r="I91" s="71" t="s">
+        <v>498</v>
+      </c>
+      <c r="J91" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K91" s="70"/>
       <c r="L91" s="70" t="s">
@@ -12426,32 +12676,36 @@
       <c r="Z91" s="14"/>
       <c r="AA91" s="14"/>
     </row>
-    <row r="92" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:27" ht="57.75" x14ac:dyDescent="0.25">
       <c r="A92" s="70">
-        <v>82</v>
-      </c>
-      <c r="B92" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C92" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D92" s="70"/>
-      <c r="E92" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F92" s="70"/>
-      <c r="G92" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H92" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I92" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J92" s="70" t="s">
-        <v>60</v>
+        <v>89</v>
+      </c>
+      <c r="B92" s="71" t="s">
+        <v>486</v>
+      </c>
+      <c r="C92" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E92" s="71" t="s">
+        <v>500</v>
+      </c>
+      <c r="F92" s="71" t="s">
+        <v>131</v>
+      </c>
+      <c r="G92" s="71" t="s">
+        <v>499</v>
+      </c>
+      <c r="H92" s="71" t="s">
+        <v>501</v>
+      </c>
+      <c r="I92" s="71" t="s">
+        <v>501</v>
+      </c>
+      <c r="J92" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K92" s="70"/>
       <c r="L92" s="70" t="s">
@@ -12473,29 +12727,31 @@
       <c r="Z92" s="14"/>
       <c r="AA92" s="14"/>
     </row>
-    <row r="93" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A93" s="70">
-        <v>83</v>
-      </c>
-      <c r="B93" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C93" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D93" s="70"/>
-      <c r="E93" s="70" t="s">
-        <v>282</v>
+        <v>90</v>
+      </c>
+      <c r="B93" s="71" t="s">
+        <v>487</v>
+      </c>
+      <c r="C93" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D93" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E93" s="71" t="s">
+        <v>502</v>
       </c>
       <c r="F93" s="70"/>
-      <c r="G93" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H93" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I93" s="70" t="s">
-        <v>285</v>
+      <c r="G93" s="71" t="s">
+        <v>503</v>
+      </c>
+      <c r="H93" s="71" t="s">
+        <v>504</v>
+      </c>
+      <c r="I93" s="71" t="s">
+        <v>505</v>
       </c>
       <c r="J93" s="70" t="s">
         <v>60</v>
@@ -12520,29 +12776,31 @@
       <c r="Z93" s="14"/>
       <c r="AA93" s="14"/>
     </row>
-    <row r="94" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:27" ht="86.25" x14ac:dyDescent="0.25">
       <c r="A94" s="70">
-        <v>84</v>
-      </c>
-      <c r="B94" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C94" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D94" s="70"/>
-      <c r="E94" s="70" t="s">
-        <v>282</v>
+        <v>91</v>
+      </c>
+      <c r="B94" s="71" t="s">
+        <v>488</v>
+      </c>
+      <c r="C94" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D94" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E94" s="71" t="s">
+        <v>506</v>
       </c>
       <c r="F94" s="70"/>
-      <c r="G94" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H94" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I94" s="70" t="s">
-        <v>285</v>
+      <c r="G94" s="71" t="s">
+        <v>507</v>
+      </c>
+      <c r="H94" s="71" t="s">
+        <v>508</v>
+      </c>
+      <c r="I94" s="71" t="s">
+        <v>509</v>
       </c>
       <c r="J94" s="70" t="s">
         <v>60</v>
@@ -12567,29 +12825,31 @@
       <c r="Z94" s="14"/>
       <c r="AA94" s="14"/>
     </row>
-    <row r="95" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:27" ht="100.5" x14ac:dyDescent="0.25">
       <c r="A95" s="70">
-        <v>85</v>
-      </c>
-      <c r="B95" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C95" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D95" s="70"/>
-      <c r="E95" s="70" t="s">
-        <v>282</v>
+        <v>92</v>
+      </c>
+      <c r="B95" s="71" t="s">
+        <v>489</v>
+      </c>
+      <c r="C95" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D95" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E95" s="71" t="s">
+        <v>510</v>
       </c>
       <c r="F95" s="70"/>
-      <c r="G95" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H95" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I95" s="70" t="s">
-        <v>285</v>
+      <c r="G95" s="71" t="s">
+        <v>511</v>
+      </c>
+      <c r="H95" s="71" t="s">
+        <v>512</v>
+      </c>
+      <c r="I95" s="71" t="s">
+        <v>513</v>
       </c>
       <c r="J95" s="70" t="s">
         <v>60</v>
@@ -12614,32 +12874,36 @@
       <c r="Z95" s="14"/>
       <c r="AA95" s="14"/>
     </row>
-    <row r="96" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:27" ht="72" x14ac:dyDescent="0.25">
       <c r="A96" s="70">
-        <v>86</v>
-      </c>
-      <c r="B96" s="70" t="s">
-        <v>287</v>
-      </c>
-      <c r="C96" s="70" t="s">
-        <v>281</v>
-      </c>
-      <c r="D96" s="70"/>
-      <c r="E96" s="70" t="s">
-        <v>282</v>
-      </c>
-      <c r="F96" s="70"/>
-      <c r="G96" s="70" t="s">
-        <v>283</v>
-      </c>
-      <c r="H96" s="70" t="s">
-        <v>284</v>
-      </c>
-      <c r="I96" s="70" t="s">
-        <v>285</v>
-      </c>
-      <c r="J96" s="70" t="s">
-        <v>60</v>
+        <v>93</v>
+      </c>
+      <c r="B96" s="71" t="s">
+        <v>490</v>
+      </c>
+      <c r="C96" s="71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D96" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="E96" s="71" t="s">
+        <v>514</v>
+      </c>
+      <c r="F96" s="71" t="s">
+        <v>515</v>
+      </c>
+      <c r="G96" s="71" t="s">
+        <v>516</v>
+      </c>
+      <c r="H96" s="71" t="s">
+        <v>517</v>
+      </c>
+      <c r="I96" s="71" t="s">
+        <v>517</v>
+      </c>
+      <c r="J96" s="71" t="s">
+        <v>52</v>
       </c>
       <c r="K96" s="70"/>
       <c r="L96" s="70" t="s">
@@ -12663,7 +12927,7 @@
     </row>
     <row r="97" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A97" s="70">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B97" s="70" t="s">
         <v>287</v>
@@ -12710,7 +12974,7 @@
     </row>
     <row r="98" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A98" s="70">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B98" s="70" t="s">
         <v>287</v>
@@ -12757,7 +13021,7 @@
     </row>
     <row r="99" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A99" s="70">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B99" s="70" t="s">
         <v>287</v>
@@ -12804,7 +13068,7 @@
     </row>
     <row r="100" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A100" s="70">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B100" s="70" t="s">
         <v>287</v>
@@ -12851,7 +13115,7 @@
     </row>
     <row r="101" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A101" s="70">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B101" s="70" t="s">
         <v>287</v>
@@ -12898,7 +13162,7 @@
     </row>
     <row r="102" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A102" s="70">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B102" s="70" t="s">
         <v>287</v>
@@ -12945,7 +13209,7 @@
     </row>
     <row r="103" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A103" s="70">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B103" s="70" t="s">
         <v>287</v>
@@ -12992,7 +13256,7 @@
     </row>
     <row r="104" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A104" s="70">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B104" s="70" t="s">
         <v>287</v>
@@ -13039,7 +13303,7 @@
     </row>
     <row r="105" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A105" s="70">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B105" s="70" t="s">
         <v>287</v>
@@ -13086,7 +13350,7 @@
     </row>
     <row r="106" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A106" s="70">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B106" s="70" t="s">
         <v>287</v>
@@ -13133,7 +13397,7 @@
     </row>
     <row r="107" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A107" s="70">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B107" s="70" t="s">
         <v>287</v>
@@ -13180,7 +13444,7 @@
     </row>
     <row r="108" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A108" s="70">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B108" s="70" t="s">
         <v>287</v>
@@ -13227,7 +13491,7 @@
     </row>
     <row r="109" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A109" s="70">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B109" s="70" t="s">
         <v>287</v>
@@ -13274,7 +13538,7 @@
     </row>
     <row r="110" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A110" s="70">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B110" s="70" t="s">
         <v>287</v>
@@ -13321,7 +13585,7 @@
     </row>
     <row r="111" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
       <c r="A111" s="70">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B111" s="70" t="s">
         <v>287</v>
@@ -13366,9 +13630,52 @@
       <c r="Z111" s="14"/>
       <c r="AA111" s="14"/>
     </row>
-    <row r="112" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F112" s="12"/>
-      <c r="M112" s="69"/>
+    <row r="112" spans="1:27" ht="44.25" x14ac:dyDescent="0.25">
+      <c r="A112" s="70">
+        <v>109</v>
+      </c>
+      <c r="B112" s="70" t="s">
+        <v>287</v>
+      </c>
+      <c r="C112" s="70" t="s">
+        <v>281</v>
+      </c>
+      <c r="D112" s="70"/>
+      <c r="E112" s="70" t="s">
+        <v>282</v>
+      </c>
+      <c r="F112" s="70"/>
+      <c r="G112" s="70" t="s">
+        <v>283</v>
+      </c>
+      <c r="H112" s="70" t="s">
+        <v>284</v>
+      </c>
+      <c r="I112" s="70" t="s">
+        <v>285</v>
+      </c>
+      <c r="J112" s="70" t="s">
+        <v>60</v>
+      </c>
+      <c r="K112" s="70"/>
+      <c r="L112" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="M112" s="72"/>
+      <c r="N112" s="70"/>
+      <c r="O112" s="70"/>
+      <c r="P112" s="70"/>
+      <c r="Q112" s="70"/>
+      <c r="R112" s="70"/>
+      <c r="S112" s="70"/>
+      <c r="T112" s="70"/>
+      <c r="U112" s="14"/>
+      <c r="V112" s="14"/>
+      <c r="W112" s="14"/>
+      <c r="X112" s="14"/>
+      <c r="Y112" s="14"/>
+      <c r="Z112" s="14"/>
+      <c r="AA112" s="14"/>
     </row>
     <row r="113" spans="6:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F113" s="12"/>
@@ -13404,6 +13711,7 @@
     </row>
     <row r="121" spans="6:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F121" s="12"/>
+      <c r="M121" s="69"/>
     </row>
     <row r="122" spans="6:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F122" s="12"/>
@@ -16062,6 +16370,9 @@
     </row>
     <row r="1007" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1007" s="12"/>
+    </row>
+    <row r="1008" spans="6:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F1008" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>